<commit_message>
update to IO list
</commit_message>
<xml_diff>
--- a/DOCS/labsis.xlsx
+++ b/DOCS/labsis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canelas_t1\Desktop\tiag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canelas_t1\source\vscode-gits\Robo-Dragster---LABSIS\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD4BD7B-5943-418F-8B92-62E6B95AEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86572DA4-802B-4240-A4F9-0F1FAF696E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EA0A12A-CF69-4697-9CAE-57BE44130B7C}"/>
   </bookViews>
@@ -705,7 +705,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -789,12 +789,37 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -818,38 +843,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1188,21 +1181,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C434037-083B-4F39-96AF-08E80CD6FAD3}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="I6" zoomScale="105" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12:V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1215,7 +1208,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1238,12 +1231,12 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="38" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="7">
@@ -1271,12 +1264,12 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="32"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="5">
         <v>1</v>
       </c>
@@ -1302,7 +1295,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1332,7 +1325,7 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1373,7 +1366,7 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1414,24 +1407,24 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="36">
         <v>5</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="51" t="s">
+      <c r="H8" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="52" t="s">
+      <c r="I8" s="37" t="s">
         <v>27</v>
       </c>
       <c r="J8" s="2"/>
@@ -1458,21 +1451,21 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="F9" s="41">
+      <c r="F9" s="4">
         <v>6</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="4" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="2"/>
@@ -1480,7 +1473,7 @@
       <c r="M9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="45" t="s">
         <v>86</v>
       </c>
       <c r="Q9" s="2" t="s">
@@ -1503,22 +1496,21 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43">
+      <c r="F10" s="3">
         <v>7</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J10" s="2"/>
@@ -1526,7 +1518,7 @@
       <c r="M10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="37"/>
+      <c r="P10" s="46"/>
       <c r="Q10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1545,22 +1537,21 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43">
+      <c r="F11" s="3">
         <v>8</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="J11" s="2"/>
@@ -1568,7 +1559,7 @@
       <c r="M11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="37"/>
+      <c r="P11" s="46"/>
       <c r="Q11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1587,24 +1578,24 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="31">
         <v>9</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="32" t="s">
         <v>39</v>
       </c>
       <c r="J12" s="2"/>
@@ -1612,7 +1603,7 @@
       <c r="M12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="38"/>
+      <c r="P12" s="47"/>
       <c r="Q12" s="2" t="s">
         <v>59</v>
       </c>
@@ -1627,28 +1618,28 @@
       <c r="V12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="W12" s="31" t="s">
+      <c r="W12" s="38" t="s">
         <v>83</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="48">
+      <c r="E13" s="41"/>
+      <c r="F13" s="33">
         <v>10</v>
       </c>
-      <c r="G13" s="48" t="s">
+      <c r="G13" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="H13" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="49" t="s">
+      <c r="I13" s="34" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="2"/>
@@ -1656,7 +1647,7 @@
       <c r="M13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P13" s="39" t="s">
+      <c r="P13" s="48" t="s">
         <v>82</v>
       </c>
       <c r="Q13" s="2" t="s">
@@ -1673,11 +1664,11 @@
       <c r="V13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="W13" s="32"/>
+      <c r="W13" s="39"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1699,7 +1690,7 @@
       <c r="M14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P14" s="40"/>
+      <c r="P14" s="49"/>
       <c r="Q14" s="2" t="s">
         <v>64</v>
       </c>
@@ -1718,7 +1709,7 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1738,7 +1729,9 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="3"/>
-      <c r="P15" s="2"/>
+      <c r="P15" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="Q15" s="2" t="s">
         <v>109</v>
       </c>
@@ -1759,7 +1752,7 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1799,12 +1792,12 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="42" t="s">
         <v>86</v>
       </c>
       <c r="F17" s="7">
@@ -1839,12 +1832,12 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="34"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="4">
         <v>15</v>
       </c>
@@ -1859,9 +1852,6 @@
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="P18" s="27" t="s">
-        <v>88</v>
-      </c>
       <c r="Q18" s="2" t="s">
         <v>105</v>
       </c>
@@ -1882,7 +1872,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>88</v>
       </c>
@@ -1891,7 +1881,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="34"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="4">
         <v>16</v>
       </c>
@@ -1920,13 +1910,13 @@
       <c r="V19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="W19" s="31" t="s">
+      <c r="W19" s="38" t="s">
         <v>3</v>
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +1925,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="35"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="5">
         <v>17</v>
       </c>
@@ -1965,11 +1955,11 @@
       <c r="V20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="W20" s="32"/>
+      <c r="W20" s="39"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +1968,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="38" t="s">
         <v>82</v>
       </c>
       <c r="F21" s="7">
@@ -2006,7 +1996,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2005,7 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="32"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="5">
         <v>19</v>
       </c>
@@ -2041,7 +2031,7 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2062,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
@@ -2103,7 +2093,7 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>4</v>
       </c>
@@ -2139,7 +2129,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26">
         <f>SUM(B19:B25)</f>
         <v>17</v>
@@ -2184,7 +2174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E27" s="11"/>
       <c r="F27" s="12">
         <v>24</v>
@@ -2213,7 +2203,7 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E28" s="23"/>
       <c r="F28" s="3">
         <v>25</v>
@@ -2241,7 +2231,7 @@
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E29" s="23"/>
       <c r="F29" s="3">
         <v>26</v>
@@ -2270,7 +2260,7 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="24"/>
       <c r="F30" s="6">
         <v>27</v>
@@ -2297,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2316,7 +2306,7 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -2332,7 +2322,7 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -2350,7 +2340,7 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -2366,7 +2356,7 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>2</v>
       </c>
@@ -2382,12 +2372,12 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>91</v>
       </c>
@@ -2407,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>92</v>
       </c>
@@ -2431,7 +2421,7 @@
       </c>
       <c r="V38" s="29"/>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>93</v>
       </c>
@@ -2439,7 +2429,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="Q41" s="2" t="s">
         <v>114</v>
       </c>
@@ -2450,7 +2440,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="P42" s="2" t="s">
         <v>120</v>
       </c>
@@ -2461,7 +2451,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="Q43" t="s">
         <v>122</v>
       </c>

</xml_diff>